<commit_message>
Correction table des états
</commit_message>
<xml_diff>
--- a/Labo_7_acqui_pos/Table_etats.xlsx
+++ b/Labo_7_acqui_pos/Table_etats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEIG\S5\CSN\Labo_7_acqui_pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC573BD6-9736-4D05-BCB3-61DC1EF129E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560C563D-BB31-48E6-8262-673C8E3B6F9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,8 +446,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -455,34 +479,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +768,7 @@
   <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:M22"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,45 +782,45 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="23" t="s">
+      <c r="F3" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="21"/>
-      <c r="M3" s="22"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="29"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="27" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="22">
         <v>11</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="23" t="s">
         <v>29</v>
       </c>
       <c r="K4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="29" t="s">
+      <c r="L4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="24" t="s">
         <v>26</v>
       </c>
       <c r="P4" s="14" t="s">
@@ -997,7 +997,7 @@
         <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>35</v>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="6:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F17" s="15" t="s">
         <v>19</v>
       </c>

</xml_diff>